<commit_message>
added headings to pack parts of draft sheet
</commit_message>
<xml_diff>
--- a/archive/100.xlsx
+++ b/archive/100.xlsx
@@ -494,6 +494,26 @@
           <t>Nenni</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>shinydog</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>big big big big dumps</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Alexotl</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Nenni</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="inlineStr">

</xml_diff>